<commit_message>
Added few more teams entry in input file
</commit_message>
<xml_diff>
--- a/input_migration/String-Replacement-Teams-Only.xlsx
+++ b/input_migration/String-Replacement-Teams-Only.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gaurav K\GIT Repo\production\input_migration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E33DFCD-4D98-4C62-A362-9EE734252C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A9BE52-BCB4-48CC-9B23-6AD5881D85F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="71">
   <si>
     <t>Full Repository Name</t>
   </si>
@@ -63,9 +63,6 @@
     <t>fourthgithubrepo</t>
   </si>
   <si>
-    <t>fifthgithubrepo</t>
-  </si>
-  <si>
     <t>canopy</t>
   </si>
   <si>
@@ -198,7 +195,49 @@
     <t>gk-aks-Digital/fourthgithubrepo</t>
   </si>
   <si>
-    <t>gk-aks-Digital/fifthgithubrepo</t>
+    <t>gk-aks-Digital/production</t>
+  </si>
+  <si>
+    <t>production</t>
+  </si>
+  <si>
+    <t>dotcom</t>
+  </si>
+  <si>
+    <t>platform</t>
+  </si>
+  <si>
+    <t>front-end-platform</t>
+  </si>
+  <si>
+    <t>gk-aks-Digital/dotcom</t>
+  </si>
+  <si>
+    <t>gk-aks-Digital/platform</t>
+  </si>
+  <si>
+    <t>gk-aks-Digital/front-end-platform</t>
+  </si>
+  <si>
+    <t>dotcom-write</t>
+  </si>
+  <si>
+    <t>platform-write</t>
+  </si>
+  <si>
+    <t>frontend-platform-write</t>
+  </si>
+  <si>
+    <t>gk-aks-CONFIDENTIAL\my-account-write</t>
+  </si>
+  <si>
+    <t>gk-aks-CONFIDENTIAL\dotcom-write</t>
+  </si>
+  <si>
+    <t>gk-aks-CONFIDENTIAL\platform-write</t>
+  </si>
+  <si>
+    <t>gk-aks-CONFIDENTIAL\frontend-platform-write</t>
   </si>
 </sst>
 </file>
@@ -516,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="A1:H16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -562,392 +601,522 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
         <v>57</v>
       </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" t="s">
         <v>57</v>
       </c>
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" t="s">
         <v>57</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>12</v>
       </c>
-      <c r="C14" t="s">
-        <v>13</v>
-      </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" t="s">
         <v>32</v>
       </c>
-      <c r="G14" t="s">
-        <v>33</v>
-      </c>
       <c r="H14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" t="s">
         <v>57</v>
       </c>
-      <c r="B15" t="s">
-        <v>12</v>
-      </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
         <v>57</v>
       </c>
-      <c r="B16" t="s">
-        <v>12</v>
-      </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H16" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" t="s">
+        <v>65</v>
+      </c>
+      <c r="H20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the Coln names
</commit_message>
<xml_diff>
--- a/input_migration/String-Replacement-Teams-Only.xlsx
+++ b/input_migration/String-Replacement-Teams-Only.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gaurav K\GIT Repo\production\input_migration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A9BE52-BCB4-48CC-9B23-6AD5881D85F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341F08A0-7215-405C-9484-18D4F554902A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,9 +36,6 @@
     <t>Team/User in Digital</t>
   </si>
   <si>
-    <t>Full Team Name in Digital</t>
-  </si>
-  <si>
     <t>Classification</t>
   </si>
   <si>
@@ -48,9 +45,6 @@
     <t>Team in EMU</t>
   </si>
   <si>
-    <t>Full Team Name in EMU</t>
-  </si>
-  <si>
     <t>firstgithubrepo</t>
   </si>
   <si>
@@ -238,13 +232,19 @@
   </si>
   <si>
     <t>gk-aks-CONFIDENTIAL\frontend-platform-write</t>
+  </si>
+  <si>
+    <t>Full Team Name Digital</t>
+  </si>
+  <si>
+    <t>Full Team Name EMU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,13 +252,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -273,8 +287,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,7 +573,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -574,549 +589,549 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
+      <c r="H1" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
         <v>28</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>30</v>
       </c>
-      <c r="G2" t="s">
-        <v>32</v>
-      </c>
       <c r="H2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
         <v>29</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>31</v>
       </c>
-      <c r="G3" t="s">
-        <v>33</v>
-      </c>
       <c r="H3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
         <v>29</v>
       </c>
-      <c r="F4" t="s">
-        <v>31</v>
-      </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
         <v>28</v>
       </c>
-      <c r="F5" t="s">
-        <v>30</v>
-      </c>
       <c r="G5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
         <v>28</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>30</v>
       </c>
-      <c r="G6" t="s">
-        <v>32</v>
-      </c>
       <c r="H6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
         <v>28</v>
       </c>
-      <c r="F7" t="s">
-        <v>30</v>
-      </c>
       <c r="G7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
         <v>28</v>
       </c>
-      <c r="F8" t="s">
-        <v>30</v>
-      </c>
       <c r="G8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
         <v>28</v>
       </c>
-      <c r="F9" t="s">
-        <v>30</v>
-      </c>
       <c r="G9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" t="s">
         <v>28</v>
       </c>
-      <c r="F10" t="s">
-        <v>30</v>
-      </c>
       <c r="G10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" t="s">
         <v>28</v>
       </c>
-      <c r="F11" t="s">
-        <v>30</v>
-      </c>
       <c r="G11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" t="s">
         <v>29</v>
       </c>
-      <c r="F12" t="s">
-        <v>31</v>
-      </c>
       <c r="G12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" t="s">
         <v>27</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>29</v>
       </c>
-      <c r="F13" t="s">
-        <v>31</v>
-      </c>
       <c r="G13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" t="s">
         <v>29</v>
       </c>
-      <c r="F14" t="s">
-        <v>31</v>
-      </c>
       <c r="G14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" t="s">
         <v>29</v>
       </c>
-      <c r="F15" t="s">
-        <v>31</v>
-      </c>
       <c r="G15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" t="s">
         <v>29</v>
       </c>
-      <c r="F16" t="s">
-        <v>31</v>
-      </c>
       <c r="G16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" t="s">
         <v>29</v>
       </c>
-      <c r="F17" t="s">
-        <v>31</v>
-      </c>
       <c r="G17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" t="s">
         <v>29</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>31</v>
       </c>
-      <c r="G18" t="s">
-        <v>33</v>
-      </c>
       <c r="H18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s">
         <v>56</v>
       </c>
-      <c r="B19" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" t="s">
-        <v>58</v>
-      </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E19" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" t="s">
         <v>29</v>
       </c>
-      <c r="F19" t="s">
-        <v>31</v>
-      </c>
       <c r="G19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s">
         <v>57</v>
       </c>
-      <c r="C20" t="s">
-        <v>59</v>
-      </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" t="s">
         <v>29</v>
       </c>
-      <c r="F20" t="s">
-        <v>31</v>
-      </c>
       <c r="G20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" t="s">
         <v>29</v>
       </c>
-      <c r="F21" t="s">
-        <v>31</v>
-      </c>
       <c r="G21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>